<commit_message>
changes on excel file
</commit_message>
<xml_diff>
--- a/ProjectObjects.xlsx
+++ b/ProjectObjects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VFS\Term1\Programming1\Assignment3\Clicker_Heros_Console\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VFS\Term1\Programming1\Assignment3\Clicker_Hero\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Program</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>DamagePerClick</t>
+  </si>
+  <si>
+    <t>Simple Screen</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K13"/>
+  <dimension ref="A2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1396,53 +1399,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+    <row r="11" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
+    <row r="13" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+    <row r="14" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="15" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>